<commit_message>
Inicio de clases :D
</commit_message>
<xml_diff>
--- a/NOTAS FINALES.xlsx
+++ b/NOTAS FINALES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lusca\Documents\facultad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDE74A0-23FA-40C9-AA91-C536EC30A267}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589654A8-2D56-4DAD-94F6-78EAACA3C5D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44DCED10-E3F3-460B-AC11-D0A6D3D8F230}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>QUIMICA GENERAL</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>PROGRAMACION I</t>
+  </si>
+  <si>
+    <t>DISEÑO DE SISTEMAS</t>
   </si>
 </sst>
 </file>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAD7D97-593E-4F02-A8E7-271229031F2F}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,8 +624,8 @@
         <v>10</v>
       </c>
       <c r="F2" s="5">
-        <f>(SUM(E2:E26))/A26</f>
-        <v>9.08</v>
+        <f>(SUM(E2:E27))/A26</f>
+        <v>9.48</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1036,8 +1039,25 @@
         <v>10</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2031</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="6">
+        <v>44265</v>
+      </c>
+      <c r="E27" s="1">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E26">
+  <conditionalFormatting sqref="E2:E27">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
Seguridad I y notas
</commit_message>
<xml_diff>
--- a/NOTAS FINALES.xlsx
+++ b/NOTAS FINALES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lusca\Documents\facultad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C723C12-7EE2-49E8-A1D1-BEC1C55150EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A16A3E2-8288-400B-AA0D-B9515E92D42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44DCED10-E3F3-460B-AC11-D0A6D3D8F230}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>QUIMICA GENERAL</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>COMPUTACION II</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>SEGURIDAD INFORMATICA I</t>
   </si>
 </sst>
 </file>
@@ -218,7 +224,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -230,6 +236,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -575,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAD7D97-593E-4F02-A8E7-271229031F2F}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,11 +595,11 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -609,8 +618,12 @@
       <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -627,11 +640,18 @@
         <v>10</v>
       </c>
       <c r="F2" s="5">
-        <f>(SUM(E2:E28))/A28</f>
-        <v>9.1481481481481488</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <f>(SUM(E2:E29))/A28</f>
+        <v>9.481481481481481</v>
+      </c>
+      <c r="G2">
+        <f>(A29/47)*100</f>
+        <v>59.574468085106382</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -648,7 +668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -665,7 +685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -682,7 +702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -699,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -716,7 +736,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -733,7 +753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -750,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -767,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -784,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -801,7 +821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -818,7 +838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -835,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -852,7 +872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1076,8 +1096,28 @@
         <v>10</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2044</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="6">
+        <v>44414</v>
+      </c>
+      <c r="E29" s="1">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E28">
+  <mergeCells count="1">
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
Muchas actualizaciones previo estudio febrero
</commit_message>
<xml_diff>
--- a/NOTAS FINALES.xlsx
+++ b/NOTAS FINALES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Lucas\Documents\facultad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8564A8BD-A8E1-4394-A5E8-E4CD9F869FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE63C34-94B1-4550-815D-29BE2AC506F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>N°</t>
   </si>
@@ -149,6 +149,27 @@
   </si>
   <si>
     <t>PROGRAMACION II</t>
+  </si>
+  <si>
+    <t>INGENIERIA DE SOFTWARE APLICADA</t>
+  </si>
+  <si>
+    <t>NO OFICIAL</t>
+  </si>
+  <si>
+    <t>AÑOS</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>QUEDAN</t>
+  </si>
+  <si>
+    <t>CANTIDAD AÑO</t>
+  </si>
+  <si>
+    <t>PROMEDIO QUEDAN</t>
   </si>
 </sst>
 </file>
@@ -158,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -189,8 +210,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +243,19 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -239,33 +278,199 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Excel Built-in Calculation" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,583 +882,774 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="10" width="9.42578125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="17" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="6">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="7">
         <v>43283</v>
       </c>
-      <c r="E2" s="3">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="E2" s="6">
+        <v>10</v>
+      </c>
+      <c r="F2" s="8">
         <f>(SUM(E2:E83))/COUNT(A2:A85)</f>
-        <v>9.193548387096774</v>
-      </c>
-      <c r="G2" s="6">
+        <v>9.21875</v>
+      </c>
+      <c r="G2" s="9">
         <f>(COUNT(A2:A67)/50)</f>
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="6">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="7">
         <v>43283</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="6">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>43283</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="6">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7">
         <v>43426</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="6">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="7">
         <v>43427</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="7">
         <v>43446</v>
       </c>
-      <c r="E7" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E7" s="6">
+        <v>10</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="7">
         <v>43451</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="K8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="7">
         <v>43515</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="K9" s="5">
+        <v>2018</v>
+      </c>
+      <c r="L9" s="10">
+        <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K9))</f>
+        <v>7</v>
+      </c>
+      <c r="M9" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="N9" s="10">
+        <f>M9-L9</f>
+        <v>2</v>
+      </c>
+      <c r="O9" s="23">
+        <f>SUM(L9:L12)/COUNT(L9:L12)</f>
+        <v>8</v>
+      </c>
+      <c r="P9" s="21">
+        <f>SUM(N9:N12)/COUNT(N9:N12)</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
         <v>2025</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="7">
         <v>43810</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="K10" s="5">
+        <v>2019</v>
+      </c>
+      <c r="L10" s="10">
+        <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K10))</f>
+        <v>9</v>
+      </c>
+      <c r="M10" s="10">
+        <v>10</v>
+      </c>
+      <c r="N10" s="10">
+        <f t="shared" ref="N10:N13" si="0">M10-L10</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="24"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
         <v>2020</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="7">
         <v>43643</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="K11" s="5">
+        <v>2020</v>
+      </c>
+      <c r="L11" s="10">
+        <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K11))</f>
+        <v>7</v>
+      </c>
+      <c r="M11" s="10">
+        <v>9</v>
+      </c>
+      <c r="N11" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O11" s="24"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="6">
         <v>2022</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="7">
         <v>43648</v>
       </c>
-      <c r="E12" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="E12" s="6">
+        <v>10</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="K12" s="5">
+        <v>2021</v>
+      </c>
+      <c r="L12" s="10">
+        <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K12))</f>
+        <v>9</v>
+      </c>
+      <c r="M12" s="10">
+        <v>11</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O12" s="24"/>
+      <c r="P12" s="11"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="6">
         <v>2040</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="7">
         <v>43677</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="K13" s="15">
+        <v>2022</v>
+      </c>
+      <c r="L13" s="18">
+        <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K13))</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="18">
+        <v>11</v>
+      </c>
+      <c r="N13" s="18">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="6">
         <v>2023</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="7">
         <v>43725</v>
       </c>
-      <c r="E14" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="E14" s="6">
+        <v>10</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="6">
         <v>2028</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="7">
         <v>43790</v>
       </c>
-      <c r="E15" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="E15" s="6">
+        <v>10</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="6">
         <v>2024</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="7">
         <v>43794</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="6">
         <v>2027</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="7">
         <v>43810</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="6">
         <v>2026</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="7">
         <v>43882</v>
       </c>
-      <c r="E18" s="3">
-        <v>10</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="E18" s="6">
+        <v>10</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="6">
         <v>2032</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="7">
         <v>43903</v>
       </c>
-      <c r="E19" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="E19" s="6">
+        <v>10</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="6">
         <v>2031</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="7">
         <v>44013</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="6">
         <v>2033</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="7">
         <v>44046</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="6">
         <v>2054</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="7">
         <v>44160</v>
       </c>
-      <c r="E22" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="E22" s="6">
+        <v>10</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="6">
         <v>2037</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="7">
         <v>44161</v>
       </c>
-      <c r="E23" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="E23" s="6">
+        <v>10</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="6">
         <v>2035</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="7">
         <v>44180</v>
       </c>
-      <c r="E24" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="E24" s="6">
+        <v>10</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="6">
         <v>2030</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="7">
         <v>44244</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="6">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="F25" s="10"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="6">
         <v>2034</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="13">
         <v>44245</v>
       </c>
-      <c r="E26" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="E26" s="6">
+        <v>10</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="6">
         <v>2036</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="13">
         <v>44265</v>
       </c>
-      <c r="E27" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="E27" s="6">
+        <v>10</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="6">
         <v>2038</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="13">
         <v>44378</v>
       </c>
-      <c r="E28" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="E28" s="6">
+        <v>10</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="6">
         <v>2044</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="13">
         <v>44414</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="F29" s="10"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="10">
         <v>2404</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="13">
         <v>44454</v>
       </c>
-      <c r="E30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="E30" s="10">
+        <v>10</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="6">
         <v>2046</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="14">
         <v>44526</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="10">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="6">
         <v>2049</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="14">
         <v>44525</v>
       </c>
-      <c r="E32" s="3">
-        <v>10</v>
-      </c>
+      <c r="E32" s="6">
+        <v>10</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16">
+        <v>2080</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="17">
+        <v>44545</v>
+      </c>
+      <c r="E33" s="16">
+        <v>10</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E50">

</xml_diff>

<commit_message>
No se, muchas actualizaciones hasta que rendi organizacion
</commit_message>
<xml_diff>
--- a/NOTAS FINALES.xlsx
+++ b/NOTAS FINALES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Lucas\Documents\facultad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE63C34-94B1-4550-815D-29BE2AC506F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE1FF3D-1CEC-4743-842E-55933C5110F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>N°</t>
   </si>
@@ -94,9 +94,6 @@
     <t>ARQUIT. DE COMPUTADORAS</t>
   </si>
   <si>
-    <t>COMPUTACION</t>
-  </si>
-  <si>
     <t>ESTADISTICA APLICADA I</t>
   </si>
   <si>
@@ -170,15 +167,24 @@
   </si>
   <si>
     <t>PROMEDIO QUEDAN</t>
+  </si>
+  <si>
+    <t>INVESTIGACION OPERATIVA</t>
+  </si>
+  <si>
+    <t>TIF II</t>
+  </si>
+  <si>
+    <t>INGENIERIA DE SOFTWARE</t>
+  </si>
+  <si>
+    <t>COMPUTACION I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,7 +436,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -442,9 +448,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -452,13 +455,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -467,7 +465,7 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -882,11 +880,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,19 +937,19 @@
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="12">
         <v>43283</v>
       </c>
       <c r="E2" s="6">
         <v>10</v>
       </c>
-      <c r="F2" s="8">
-        <f>(SUM(E2:E83))/COUNT(A2:A85)</f>
-        <v>9.21875</v>
-      </c>
-      <c r="G2" s="9">
-        <f>(COUNT(A2:A67)/50)</f>
-        <v>0.64</v>
+      <c r="F2" s="7">
+        <f>(SUM(E2:E85))/COUNT(A2:A85)</f>
+        <v>9.2285714285714278</v>
+      </c>
+      <c r="G2" s="8">
+        <f>(COUNT(A2:A85)/50)</f>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -964,14 +962,14 @@
       <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="12">
         <v>43283</v>
       </c>
       <c r="E3" s="6">
         <v>9</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -983,14 +981,14 @@
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="12">
         <v>43283</v>
       </c>
       <c r="E4" s="6">
         <v>9</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -1002,14 +1000,14 @@
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="12">
         <v>43426</v>
       </c>
       <c r="E5" s="6">
         <v>8</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1021,14 +1019,14 @@
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="12">
         <v>43427</v>
       </c>
       <c r="E6" s="6">
         <v>9</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:16" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
@@ -1040,14 +1038,14 @@
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="12">
         <v>43446</v>
       </c>
       <c r="E7" s="6">
         <v>10</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1059,31 +1057,31 @@
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="12">
         <v>43451</v>
       </c>
       <c r="E8" s="6">
         <v>8</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
       <c r="K8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="O8" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1096,35 +1094,35 @@
       <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="12">
         <v>43515</v>
       </c>
       <c r="E9" s="6">
         <v>8</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
       <c r="K9" s="5">
         <v>2018</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="9">
         <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K9))</f>
         <v>7</v>
       </c>
-      <c r="M9" s="10">
-        <v>9</v>
-      </c>
-      <c r="N9" s="10">
+      <c r="M9" s="9">
+        <v>8</v>
+      </c>
+      <c r="N9" s="9">
         <f>M9-L9</f>
-        <v>2</v>
-      </c>
-      <c r="O9" s="23">
-        <f>SUM(L9:L12)/COUNT(L9:L12)</f>
-        <v>8</v>
-      </c>
-      <c r="P9" s="21">
+        <v>1</v>
+      </c>
+      <c r="O9" s="19">
+        <f>SUM(L9:L13)/COUNT(L9:L13)</f>
+        <v>7</v>
+      </c>
+      <c r="P9" s="17">
         <f>SUM(N9:N12)/COUNT(N9:N12)</f>
-        <v>1.75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1137,30 +1135,30 @@
       <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="12">
         <v>43810</v>
       </c>
       <c r="E10" s="6">
         <v>8</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10"/>
       <c r="K10" s="5">
         <v>2019</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="9">
         <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K10))</f>
         <v>9</v>
       </c>
-      <c r="M10" s="10">
-        <v>10</v>
-      </c>
-      <c r="N10" s="10">
-        <f t="shared" ref="N10:N13" si="0">M10-L10</f>
-        <v>1</v>
-      </c>
-      <c r="O10" s="24"/>
-      <c r="P10" s="11"/>
+      <c r="M10" s="9">
+        <v>10</v>
+      </c>
+      <c r="N10" s="9">
+        <f>(N9+M10)-L10</f>
+        <v>2</v>
+      </c>
+      <c r="O10" s="20"/>
+      <c r="P10" s="10"/>
     </row>
     <row r="11" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1172,30 +1170,30 @@
       <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="12">
         <v>43643</v>
       </c>
       <c r="E11" s="6">
         <v>8</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
       <c r="K11" s="5">
         <v>2020</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="9">
         <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K11))</f>
         <v>7</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>9</v>
       </c>
-      <c r="N11" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O11" s="24"/>
-      <c r="P11" s="11"/>
+      <c r="N11" s="9">
+        <f t="shared" ref="N11:N13" si="0">(N10+M11)-L11</f>
+        <v>4</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1207,30 +1205,30 @@
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="12">
         <v>43648</v>
       </c>
       <c r="E12" s="6">
         <v>10</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
       <c r="K12" s="5">
         <v>2021</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="9">
         <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K12))</f>
-        <v>9</v>
-      </c>
-      <c r="M12" s="10">
         <v>11</v>
       </c>
-      <c r="N12" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O12" s="24"/>
-      <c r="P12" s="11"/>
+      <c r="M12" s="9">
+        <v>12</v>
+      </c>
+      <c r="N12" s="9">
+        <f>(N11+M12)-L12</f>
+        <v>5</v>
+      </c>
+      <c r="O12" s="20"/>
+      <c r="P12" s="10"/>
     </row>
     <row r="13" spans="1:16" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
@@ -1242,30 +1240,30 @@
       <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="12">
         <v>43677</v>
       </c>
       <c r="E13" s="6">
         <v>9</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
-      <c r="K13" s="15">
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="K13" s="13">
         <v>2022</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="14">
         <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K13))</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="18">
+        <v>1</v>
+      </c>
+      <c r="M13" s="14">
         <v>11</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="14">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="O13" s="25"/>
-      <c r="P13" s="19"/>
+        <v>15</v>
+      </c>
+      <c r="O13" s="21"/>
+      <c r="P13" s="15"/>
     </row>
     <row r="14" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -1277,14 +1275,14 @@
       <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="12">
         <v>43725</v>
       </c>
       <c r="E14" s="6">
         <v>10</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -1294,16 +1292,16 @@
         <v>2028</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="7">
+        <v>48</v>
+      </c>
+      <c r="D15" s="12">
         <v>43790</v>
       </c>
       <c r="E15" s="6">
         <v>10</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1313,18 +1311,18 @@
         <v>2024</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="7">
+        <v>20</v>
+      </c>
+      <c r="D16" s="12">
         <v>43794</v>
       </c>
       <c r="E16" s="6">
         <v>9</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1332,18 +1330,34 @@
         <v>2027</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="7">
+        <v>21</v>
+      </c>
+      <c r="D17" s="12">
         <v>43810</v>
       </c>
       <c r="E17" s="6">
         <v>9</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="9"/>
+      <c r="G17" s="10"/>
+      <c r="K17" s="1">
+        <f>COUNTIF($E$2:$E$58,10)</f>
+        <v>17</v>
+      </c>
+      <c r="L17" s="1">
+        <f>COUNTIF($E$2:$E$58,9)</f>
+        <v>11</v>
+      </c>
+      <c r="M17" s="1">
+        <f>COUNTIF($E$2:$E$58,8)</f>
+        <v>5</v>
+      </c>
+      <c r="N17" s="1">
+        <f>COUNTIF($E$2:$E$58,7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1351,20 +1365,20 @@
         <v>2026</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="12">
+        <v>43882</v>
+      </c>
+      <c r="E18" s="6">
+        <v>10</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="7">
-        <v>43882</v>
-      </c>
-      <c r="E18" s="6">
-        <v>10</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1372,18 +1386,18 @@
         <v>2032</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="7">
+        <v>24</v>
+      </c>
+      <c r="D19" s="12">
         <v>43903</v>
       </c>
       <c r="E19" s="6">
         <v>10</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1391,18 +1405,18 @@
         <v>2031</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="7">
+        <v>25</v>
+      </c>
+      <c r="D20" s="12">
         <v>44013</v>
       </c>
       <c r="E20" s="6">
         <v>9</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="9"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1410,18 +1424,18 @@
         <v>2033</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="7">
+        <v>26</v>
+      </c>
+      <c r="D21" s="12">
         <v>44046</v>
       </c>
       <c r="E21" s="6">
         <v>7</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="9"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1429,18 +1443,18 @@
         <v>2054</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="7">
+        <v>27</v>
+      </c>
+      <c r="D22" s="12">
         <v>44160</v>
       </c>
       <c r="E22" s="6">
         <v>10</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1448,18 +1462,18 @@
         <v>2037</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="7">
+        <v>28</v>
+      </c>
+      <c r="D23" s="12">
         <v>44161</v>
       </c>
       <c r="E23" s="6">
         <v>10</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="9"/>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1467,18 +1481,18 @@
         <v>2035</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="7">
+        <v>29</v>
+      </c>
+      <c r="D24" s="12">
         <v>44180</v>
       </c>
       <c r="E24" s="6">
         <v>10</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1486,18 +1500,18 @@
         <v>2030</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="7">
+        <v>30</v>
+      </c>
+      <c r="D25" s="12">
         <v>44244</v>
       </c>
       <c r="E25" s="6">
         <v>7</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" s="9"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1505,18 +1519,18 @@
         <v>2034</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="13">
+        <v>31</v>
+      </c>
+      <c r="D26" s="12">
         <v>44245</v>
       </c>
       <c r="E26" s="6">
         <v>10</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1524,18 +1538,18 @@
         <v>2036</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="13">
+        <v>32</v>
+      </c>
+      <c r="D27" s="12">
         <v>44265</v>
       </c>
       <c r="E27" s="6">
         <v>10</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" s="9"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1543,18 +1557,18 @@
         <v>2038</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="13">
+        <v>33</v>
+      </c>
+      <c r="D28" s="12">
         <v>44378</v>
       </c>
       <c r="E28" s="6">
         <v>10</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="9"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1562,56 +1576,56 @@
         <v>2044</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="13">
+        <v>34</v>
+      </c>
+      <c r="D29" s="12">
         <v>44414</v>
       </c>
       <c r="E29" s="6">
         <v>9</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="9"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>2404</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="13">
+      <c r="C30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="12">
         <v>44454</v>
       </c>
-      <c r="E30" s="10">
-        <v>10</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="9">
+        <v>10</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="B31" s="6">
         <v>2046</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="14">
+      <c r="C31" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="12">
         <v>44526</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="9">
         <v>9</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F31" s="9"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1619,40 +1633,97 @@
         <v>2049</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="12">
+        <v>44525</v>
+      </c>
+      <c r="E32" s="6">
+        <v>10</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6">
+        <v>2080</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="14">
-        <v>44525</v>
-      </c>
-      <c r="E32" s="6">
-        <v>10</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="15">
-        <v>32</v>
-      </c>
-      <c r="B33" s="16">
-        <v>2080</v>
-      </c>
-      <c r="C33" s="16" t="s">
+      <c r="D33" s="12">
+        <v>44545</v>
+      </c>
+      <c r="E33" s="6">
+        <v>10</v>
+      </c>
+      <c r="F33" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="17">
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9">
+        <v>2047</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="12">
         <v>44545</v>
       </c>
-      <c r="E33" s="16">
-        <v>10</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="G33" s="19"/>
+      <c r="E34" s="9">
+        <v>9</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9">
+        <v>2409</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="12">
+        <v>44546</v>
+      </c>
+      <c r="E35" s="9">
+        <v>9</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9">
+        <v>2041</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="12">
+        <v>44609</v>
+      </c>
+      <c r="E36" s="9">
+        <v>10</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E50">
+  <conditionalFormatting sqref="E2:E85">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
post mesas de marzo 2022
</commit_message>
<xml_diff>
--- a/NOTAS FINALES.xlsx
+++ b/NOTAS FINALES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Lucas\Documents\facultad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE1FF3D-1CEC-4743-842E-55933C5110F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E17D515-A614-48AA-8153-7D98C409887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>N°</t>
   </si>
@@ -151,9 +151,6 @@
     <t>INGENIERIA DE SOFTWARE APLICADA</t>
   </si>
   <si>
-    <t>NO OFICIAL</t>
-  </si>
-  <si>
     <t>AÑOS</t>
   </si>
   <si>
@@ -179,13 +176,16 @@
   </si>
   <si>
     <t>COMPUTACION I</t>
+  </si>
+  <si>
+    <t>ORGANIZACIÓN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -216,15 +216,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,17 +244,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -364,81 +352,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -460,20 +382,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+  <cellStyles count="3">
     <cellStyle name="Excel Built-in Calculation" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -880,11 +831,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17:O17"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,11 +896,11 @@
       </c>
       <c r="F2" s="7">
         <f>(SUM(E2:E85))/COUNT(A2:A85)</f>
-        <v>9.2285714285714278</v>
+        <v>9.25</v>
       </c>
       <c r="G2" s="8">
         <f>(COUNT(A2:A85)/50)</f>
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1066,22 +1017,22 @@
       <c r="F8" s="9"/>
       <c r="G8" s="10"/>
       <c r="K8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="O8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1116,11 +1067,11 @@
         <f>M9-L9</f>
         <v>1</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="21">
         <f>SUM(L9:L13)/COUNT(L9:L13)</f>
-        <v>7</v>
-      </c>
-      <c r="P9" s="17">
+        <v>7.2</v>
+      </c>
+      <c r="P9" s="24">
         <f>SUM(N9:N12)/COUNT(N9:N12)</f>
         <v>3</v>
       </c>
@@ -1157,7 +1108,7 @@
         <f>(N9+M10)-L10</f>
         <v>2</v>
       </c>
-      <c r="O10" s="20"/>
+      <c r="O10" s="9"/>
       <c r="P10" s="10"/>
     </row>
     <row r="11" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1192,7 +1143,7 @@
         <f t="shared" ref="N11:N13" si="0">(N10+M11)-L11</f>
         <v>4</v>
       </c>
-      <c r="O11" s="20"/>
+      <c r="O11" s="9"/>
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1227,10 +1178,10 @@
         <f>(N11+M12)-L12</f>
         <v>5</v>
       </c>
-      <c r="O12" s="20"/>
+      <c r="O12" s="9"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1248,24 +1199,24 @@
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="10"/>
-      <c r="K13" s="13">
+      <c r="K13" s="5">
         <v>2022</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="9">
         <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K13))</f>
-        <v>1</v>
-      </c>
-      <c r="M13" s="14">
+        <v>2</v>
+      </c>
+      <c r="M13" s="9">
         <v>11</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="9">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="15"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1283,6 +1234,22 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="10"/>
+      <c r="K14" s="13">
+        <v>2023</v>
+      </c>
+      <c r="L14" s="14">
+        <f>SUMPRODUCT(--(YEAR($D$2:$D$65)=K14))</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="14">
+        <f t="shared" ref="N14" si="1">(N13+M14)-L14</f>
+        <v>14</v>
+      </c>
+      <c r="O14" s="14"/>
+      <c r="P14" s="15"/>
     </row>
     <row r="15" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -1292,7 +1259,7 @@
         <v>2028</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="12">
         <v>43790</v>
@@ -1303,7 +1270,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1322,7 +1289,7 @@
       <c r="F16" s="9"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1340,45 +1307,63 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="10"/>
-      <c r="K17" s="1">
+      <c r="K17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="18">
+        <v>10</v>
+      </c>
+      <c r="M17" s="18">
+        <v>9</v>
+      </c>
+      <c r="N17" s="18">
+        <v>8</v>
+      </c>
+      <c r="O17" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2026</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="12">
+        <v>43882</v>
+      </c>
+      <c r="E18" s="6">
+        <v>10</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="K18" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="22">
         <f>COUNTIF($E$2:$E$58,10)</f>
-        <v>17</v>
-      </c>
-      <c r="L17" s="1">
+        <v>18</v>
+      </c>
+      <c r="M18" s="22">
         <f>COUNTIF($E$2:$E$58,9)</f>
         <v>11</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N18" s="22">
         <f>COUNTIF($E$2:$E$58,8)</f>
         <v>5</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O18" s="23">
         <f>COUNTIF($E$2:$E$58,7)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6">
-        <v>2026</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="12">
-        <v>43882</v>
-      </c>
-      <c r="E18" s="6">
-        <v>10</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1397,7 +1382,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1416,7 +1401,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1435,7 +1420,7 @@
       <c r="F21" s="9"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1454,7 +1439,7 @@
       <c r="F22" s="9"/>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1473,7 +1458,7 @@
       <c r="F23" s="9"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1492,7 +1477,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1511,7 +1496,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1530,7 +1515,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1549,7 +1534,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1568,7 +1553,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1587,7 +1572,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1606,7 +1591,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1625,7 +1610,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1660,9 +1645,7 @@
       <c r="E33" s="6">
         <v>10</v>
       </c>
-      <c r="F33" s="22" t="s">
-        <v>39</v>
-      </c>
+      <c r="F33" s="9"/>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1673,7 +1656,7 @@
         <v>2047</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D34" s="12">
         <v>44545</v>
@@ -1692,7 +1675,7 @@
         <v>2409</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D35" s="12">
         <v>44546</v>
@@ -1711,7 +1694,7 @@
         <v>2041</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" s="12">
         <v>44609</v>
@@ -1722,20 +1705,59 @@
       <c r="F36" s="9"/>
       <c r="G36" s="10"/>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9">
+        <v>2043</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="12">
+        <v>44627</v>
+      </c>
+      <c r="E37" s="9">
+        <v>10</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D38" s="17"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E85">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="E2:E36 E38:E85">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="between">
       <formula>"9.01"</formula>
       <formula>9.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="between">
       <formula>6</formula>
       <formula>7.99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="between">
+      <formula>8</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>"9.01"</formula>
+      <formula>9.99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+      <formula>6</formula>
+      <formula>7.99</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
       <formula>8</formula>
       <formula>9</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mitad del semestre prácticamente
</commit_message>
<xml_diff>
--- a/NOTAS FINALES.xlsx
+++ b/NOTAS FINALES.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>N°</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t xml:space="preserve">ASEGURAMIENTO DE CALIDAD DEL SOFTWARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLANEAMIENTO Y GESTIÓN DE EMPRESAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GESTIÓN DE CALIDAD Y MEDIO AMBIENTE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIGIENE Y SEGURIDAD DEL TRABAJO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIF III</t>
   </si>
 </sst>
 </file>
@@ -172,7 +184,7 @@
   <fonts count="4">
     <font>
       <name val="Calibri"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <sz val="11.000000"/>
     </font>
     <font>
@@ -334,7 +346,7 @@
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="3" fillId="3" borderId="2" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -365,7 +377,8 @@
     <xf fontId="3" fillId="3" borderId="7" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf fontId="1" fillId="2" borderId="8" numFmtId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf fontId="1" fillId="2" borderId="9" numFmtId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Calculation" xfId="1"/>
@@ -938,11 +951,11 @@
       </c>
       <c r="F2" s="8">
         <f>(SUM(E2:E85))/COUNT(A2:A85)</f>
-        <v>9.2432432432432439</v>
+        <v>9.2439024390243905</v>
       </c>
       <c r="G2" s="9">
         <f>(COUNT(A2:A85)/50)</f>
-        <v>0.73999999999999999</v>
+        <v>0.81999999999999995</v>
       </c>
     </row>
     <row r="3" ht="15.949999999999999" customHeight="1">
@@ -1111,7 +1124,7 @@
       </c>
       <c r="O9" s="13">
         <f>SUM(L9:L13)/COUNT(L9:L13)</f>
-        <v>7.4000000000000004</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="P9" s="14">
         <f>SUM(N9:N12)/COUNT(N9:N12)</f>
@@ -1246,14 +1259,14 @@
       </c>
       <c r="L13" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M13" s="10">
         <v>11</v>
       </c>
       <c r="N13" s="10">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O13" s="10"/>
       <c r="P13" s="11"/>
@@ -1288,7 +1301,7 @@
       </c>
       <c r="N14" s="16">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O14" s="16"/>
       <c r="P14" s="17"/>
@@ -1390,11 +1403,11 @@
       </c>
       <c r="L18" s="22">
         <f>COUNTIF($E$2:$E$58,10)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M18" s="22">
         <f>COUNTIF($E$2:$E$58,9)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N18" s="22">
         <f>COUNTIF($E$2:$E$58,8)</f>
@@ -1773,7 +1786,7 @@
       <c r="B38" s="10">
         <v>2501</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="7">
@@ -1784,17 +1797,93 @@
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="11"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" s="10">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2509</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="24">
+        <v>44749</v>
+      </c>
+      <c r="E39" s="1">
+        <v>9</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="A40" s="10">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2502</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="24">
+        <v>44750</v>
+      </c>
+      <c r="E40" s="1">
+        <v>9</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" s="10">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2503</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="24">
+        <v>44750</v>
+      </c>
+      <c r="E41" s="1">
+        <v>9</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" ht="14.25">
+      <c r="A42" s="10">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2505</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="24">
+        <v>44826</v>
+      </c>
+      <c r="E42" s="1">
+        <v>10</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" operator="between" id="{00C900EF-00CE-4631-B3DA-00B600850074}">
+          <x14:cfRule type="cellIs" priority="9" operator="between" id="{00FA0095-0018-4577-95C3-006700230090}">
             <xm:f>8</xm:f>
             <xm:f>9</xm:f>
             <x14:dxf>
@@ -1809,7 +1898,7 @@
           <xm:sqref>E2:E36 E39:E85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="between" id="{004A00C4-008C-479D-9A65-003500E6008C}">
+          <x14:cfRule type="cellIs" priority="8" operator="between" id="{007400AA-00AD-48CF-BD11-00CF008D00B3}">
             <xm:f>6</xm:f>
             <xm:f>7.99</xm:f>
             <x14:dxf>
@@ -1824,7 +1913,7 @@
           <xm:sqref>E2:E36 E39:E85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="between" id="{005A00E5-0024-4719-AE59-009E002B00DD}">
+          <x14:cfRule type="cellIs" priority="7" operator="between" id="{00D000AC-000C-4EEB-9203-003E00100004}">
             <xm:f>"9.01"</xm:f>
             <xm:f>9.99</xm:f>
             <x14:dxf>
@@ -1839,7 +1928,7 @@
           <xm:sqref>E2:E36 E39:E85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00130078-0053-499E-BDA3-00F800BD0092}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{00CB00E9-00FC-433B-BB7E-0063001D00CB}">
             <xm:f>10</xm:f>
             <x14:dxf>
               <fill>
@@ -1853,7 +1942,7 @@
           <xm:sqref>E2:E36 E39:E85</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="between" id="{008900D3-0095-49FC-9F1F-00A6002E00D9}">
+          <x14:cfRule type="cellIs" priority="4" operator="between" id="{001C0091-000A-4E69-A101-00750051001F}">
             <xm:f>8</xm:f>
             <xm:f>9</xm:f>
             <x14:dxf>
@@ -1868,7 +1957,7 @@
           <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="between" id="{00730063-0014-4895-A9CB-00500009007C}">
+          <x14:cfRule type="cellIs" priority="4" operator="between" id="{001100DB-00B1-4C0D-8C4D-000700600097}">
             <xm:f>8</xm:f>
             <xm:f>9</xm:f>
             <x14:dxf>
@@ -1883,7 +1972,7 @@
           <xm:sqref>E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="between" id="{00B800B3-00F1-4F26-881B-000C0002003F}">
+          <x14:cfRule type="cellIs" priority="3" operator="between" id="{00F0007C-00CB-4A25-AE77-001F001900C1}">
             <xm:f>6</xm:f>
             <xm:f>7.99</xm:f>
             <x14:dxf>
@@ -1898,7 +1987,7 @@
           <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="between" id="{00D80060-00A9-47FF-B863-003100AB00AF}">
+          <x14:cfRule type="cellIs" priority="3" operator="between" id="{00FB00EF-001F-4DDC-B6A9-003500E000E8}">
             <xm:f>6</xm:f>
             <xm:f>7.99</xm:f>
             <x14:dxf>
@@ -1913,7 +2002,7 @@
           <xm:sqref>E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="between" id="{0018005C-00B6-499C-96E7-00E2000700D7}">
+          <x14:cfRule type="cellIs" priority="2" operator="between" id="{000500F5-0023-466E-8FCD-009200640070}">
             <xm:f>"9.01"</xm:f>
             <xm:f>9.99</xm:f>
             <x14:dxf>
@@ -1928,7 +2017,7 @@
           <xm:sqref>E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="between" id="{000100C7-0095-44C1-A159-003200AD00BF}">
+          <x14:cfRule type="cellIs" priority="2" operator="between" id="{006E00A1-0047-48AD-AC22-006C00FC0083}">
             <xm:f>"9.01"</xm:f>
             <xm:f>9.99</xm:f>
             <x14:dxf>
@@ -1943,7 +2032,7 @@
           <xm:sqref>E38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00740076-000D-45C5-9265-005A00D30097}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00730075-0097-4E8B-8A93-001B00C00060}">
             <xm:f>10</xm:f>
             <x14:dxf>
               <fill>
@@ -1957,7 +2046,7 @@
           <xm:sqref>E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{0027008F-0022-4C50-B7FA-00C100A700B8}">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{003A004F-0087-48CA-9258-009700AB0077}">
             <xm:f>10</xm:f>
             <x14:dxf>
               <fill>

</xml_diff>